<commit_message>
Add backend, frontend, and essential scripts
- Add complete backend FastAPI application
- Add Vue.js frontend with Element Plus
- Add management and testing scripts
- Add configuration files and documentation

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/bad12.xlsx
+++ b/bad12.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="109">
   <si>
     <t>最后客户消息</t>
   </si>
@@ -41,36 +41,6 @@
     <t>销售消息时间</t>
   </si>
   <si>
-    <t>SOP一级节点</t>
-  </si>
-  <si>
-    <t>SOP二级节点</t>
-  </si>
-  <si>
-    <t>SOP三级节点</t>
-  </si>
-  <si>
-    <t>SOP四级节点</t>
-  </si>
-  <si>
-    <t>SOP五级节点</t>
-  </si>
-  <si>
-    <t>SOP六级节点</t>
-  </si>
-  <si>
-    <t>SOP七级节点</t>
-  </si>
-  <si>
-    <t>SOP八级节点</t>
-  </si>
-  <si>
-    <t>SOP九级节点</t>
-  </si>
-  <si>
-    <t>匹配相似度</t>
-  </si>
-  <si>
     <t>匹配的参考话术</t>
   </si>
   <si>
@@ -308,55 +278,52 @@
     <t>2025-10-11 15:07:21</t>
   </si>
   <si>
-    <t>挖需</t>
+    <t>相似话术</t>
+  </si>
+  <si>
+    <t>{"备考卡点": "好的,现在备考时间也比较紧张啦,像咱们没有参加过考试,不太清楚，考试时候平均40秒一题，主要考察的是做题方法,咱们一定要提前规划好学习节奏,目前有没有遇到哪些备考卡点呀?"}</t>
+  </si>
+  <si>
+    <t>["主要考察的是做题方法"]</t>
+  </si>
+  <si>
+    <t>询问备考卡点</t>
+  </si>
+  <si>
+    <t>挖需 -&gt; 与首次备考国考的客户沟通 -&gt; 刚开始了解接触</t>
+  </si>
+  <si>
+    <t>挖需 -&gt; 与首次备考国考的客户沟通</t>
+  </si>
+  <si>
+    <t>同学，今天晚上就要开始上直播课了，老师整理学习档案看你是第一次备考国考，咱们开始备考复习了嘛？</t>
+  </si>
+  <si>
+    <t>强校验命中: 挖需 -&gt; 与首次备考国考的客户沟通 -&gt; 刚开始了解接触 (相似度 1.00); SOP2级节点“与首次备考国考的客户沟通”存在话术，但对话中的最高相似度仅 1.00，低于阈值 0.9</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>是</t>
+  </si>
+  <si>
+    <t>挖需 -&gt; 与首次备考国考的客户沟通 -&gt; 刚开始了解接触 -&gt; 备考卡点询问 -&gt; 邀约到课 -&gt; 上课提醒</t>
   </si>
   <si>
     <t>与首次备考国考的客户沟通</t>
   </si>
   <si>
+    <t>失败</t>
+  </si>
+  <si>
+    <t>{"邀约到课": "好的，明白，现在时间紧任务重，老师建议咱们国省考同时备考，因为考试大纲都是一样的，学难考易，上岸机会也会更多一些&lt;newline&gt;这几天直播课也会讲更多关于如何备考和考公的做题技巧方法，咱们可以先认真来听，今晚7点第一节直播课，可以按时上课吗？"}</t>
+  </si>
+  <si>
+    <t>["时间紧任务重", "国省考同时备考", "今晚7点"]</t>
+  </si>
+  <si>
     <t>刚开始了解接触</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>相似话术</t>
-  </si>
-  <si>
-    <t>{"备考卡点": "好的,现在备考时间也比较紧张啦,像咱们没有参加过考试,不太清楚，考试时候平均40秒一题，主要考察的是做题方法,咱们一定要提前规划好学习节奏,目前有没有遇到哪些备考卡点呀?"}</t>
-  </si>
-  <si>
-    <t>["主要考察的是做题方法"]</t>
-  </si>
-  <si>
-    <t>询问备考卡点</t>
-  </si>
-  <si>
-    <t>挖需 -&gt; 与首次备考国考的客户沟通 -&gt; 刚开始了解接触</t>
-  </si>
-  <si>
-    <t>挖需 -&gt; 与首次备考国考的客户沟通</t>
-  </si>
-  <si>
-    <t>同学，今天晚上就要开始上直播课了，老师整理学习档案看你是第一次备考国考，咱们开始备考复习了嘛？</t>
-  </si>
-  <si>
-    <t>强校验命中: 挖需 -&gt; 与首次备考国考的客户沟通 -&gt; 刚开始了解接触 (相似度 1.00); SOP2级节点“与首次备考国考的客户沟通”存在话术，但对话中的最高相似度仅 1.00，低于阈值 0.9</t>
-  </si>
-  <si>
-    <t>是</t>
-  </si>
-  <si>
-    <t>挖需 -&gt; 与首次备考国考的客户沟通 -&gt; 刚开始了解接触 -&gt; 备考卡点询问 -&gt; 邀约到课 -&gt; 上课提醒</t>
-  </si>
-  <si>
-    <t>失败</t>
-  </si>
-  <si>
-    <t>{"邀约到课": "好的，明白，现在时间紧任务重，老师建议咱们国省考同时备考，因为考试大纲都是一样的，学难考易，上岸机会也会更多一些&lt;newline&gt;这几天直播课也会讲更多关于如何备考和考公的做题技巧方法，咱们可以先认真来听，今晚7点第一节直播课，可以按时上课吗？"}</t>
-  </si>
-  <si>
-    <t>["时间紧任务重", "国省考同时备考", "今晚7点"]</t>
   </si>
   <si>
     <t>Cheng_Sales_705</t>
@@ -430,14 +397,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -932,133 +892,133 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1066,8 +1026,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1595,15 +1555,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:CK2"/>
+  <dimension ref="A1:CA2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="1"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:89">
+    <row r="1" s="1" customFormat="1" spans="1:79">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1841,202 +1801,172 @@
       <c r="CA1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" s="2" t="s">
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:79">
+      <c r="A2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="CJ1" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="CK1" s="2" t="s">
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:89">
-      <c r="A2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="O2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="V2" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="W2" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="X2" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="AB2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="N2" s="1">
+      <c r="AN2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AS2" s="1">
         <v>1</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="U2" s="1">
-        <v>1</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AA2" s="1">
+      <c r="AT2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AU2" s="1">
         <v>0</v>
       </c>
-      <c r="AB2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AF2" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="AG2" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="AH2" s="1">
-        <v>0.85</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AL2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AQ2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AS2" s="1">
-        <v>2</v>
-      </c>
-      <c r="AT2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="AV2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AW2" s="1" t="s">
-        <v>108</v>
+        <v>91</v>
+      </c>
+      <c r="AW2" s="1">
+        <v>0</v>
       </c>
       <c r="AX2" s="1" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="AY2" s="1">
         <v>0</v>
       </c>
       <c r="AZ2" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="BA2" s="1">
         <v>0</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="BC2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD2" s="1" t="s">
         <v>91</v>
@@ -2045,100 +1975,70 @@
         <v>0</v>
       </c>
       <c r="BF2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="BG2" s="1">
-        <v>0</v>
+        <v>91</v>
+      </c>
+      <c r="BG2" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="BH2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="BI2" s="1">
-        <v>0</v>
+        <v>94</v>
+      </c>
+      <c r="BI2" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="BJ2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="BK2" s="1">
-        <v>0</v>
+        <v>91</v>
+      </c>
+      <c r="BK2" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="BL2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="BM2" s="1">
-        <v>0</v>
+        <v>91</v>
+      </c>
+      <c r="BM2" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="BN2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="BO2" s="1">
-        <v>0</v>
+        <v>91</v>
+      </c>
+      <c r="BO2" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="BP2" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="BQ2" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="BR2" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="BS2" s="1" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="BT2" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="BU2" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="BV2" s="1" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="BW2" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="BX2" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="BY2" s="1" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="BZ2" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="CA2" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="CB2" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="CC2" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="CD2" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="CE2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="CF2" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="CG2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="CH2" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="CI2" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="CJ2" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="CK2" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>